<commit_message>
update naming format BT
</commit_message>
<xml_diff>
--- a/behavior-trees-dataset/behavior-trees-sampled-projects.xlsx
+++ b/behavior-trees-dataset/behavior-trees-sampled-projects.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Razan\Github\Behavior-Trees-in-Action\behavior-trees-dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A319A347-C82B-44FB-A376-8D477DE995D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FBEB4A-54B6-41C6-9384-2F56632F7406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{5425999F-2923-49DB-9004-1B9BE2E5E9B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Final_sampled_BT_models" sheetId="5" r:id="rId1"/>
-    <sheet name="160720_list_main_to_excute_xml" sheetId="4" r:id="rId2"/>
-    <sheet name="200320_projects_py_tree_ros" sheetId="20" r:id="rId3"/>
+    <sheet name="160720_list_main_to_excute_xml" sheetId="4" state="hidden" r:id="rId2"/>
+    <sheet name="200320_projects_py_tree_ros" sheetId="20" state="hidden" r:id="rId3"/>
     <sheet name="ipa-rar" sheetId="37" r:id="rId4"/>
     <sheet name="vislab-tecnico_vizzy_behavior" sheetId="36" r:id="rId5"/>
     <sheet name="vislab-tecnico_vizzy_playground" sheetId="35" r:id="rId6"/>

</xml_diff>